<commit_message>
fix issue 9 build for win7 was not working, etc.
</commit_message>
<xml_diff>
--- a/inst/tests/test_import.xlsx
+++ b/inst/tests/test_import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18060" windowHeight="8325" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="18060" windowHeight="8325" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="state.x77" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,12 @@
     <sheet name="formulas" sheetId="7" r:id="rId7"/>
     <sheet name="NAs" sheetId="8" r:id="rId8"/>
     <sheet name="all" sheetId="9" r:id="rId9"/>
+    <sheet name="issue9" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Price1" comment="Test a named range -- 1">deletedFields!$A$13:$C$24</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="123">
   <si>
     <t>Population</t>
   </si>
@@ -434,13 +435,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss;@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,16 +521,19 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -592,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -633,9 +637,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -647,6 +657,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -725,6 +740,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -759,6 +775,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -934,16 +951,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -969,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1015,7 @@
         <v>50708</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1027,7 +1044,7 @@
         <v>566432</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1056,7 +1073,7 @@
         <v>113417</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1102,7 @@
         <v>51945</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1114,7 +1131,7 @@
         <v>156361</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1160,7 @@
         <v>103766</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1189,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1201,7 +1218,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1230,7 +1247,7 @@
         <v>54090</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1276,7 @@
         <v>58073</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1305,7 @@
         <v>6425</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1317,7 +1334,7 @@
         <v>82677</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1346,7 +1363,7 @@
         <v>55748</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1375,7 +1392,7 @@
         <v>36097</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1404,7 +1421,7 @@
         <v>55941</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1433,7 +1450,7 @@
         <v>81787</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1462,7 +1479,7 @@
         <v>39650</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1491,7 +1508,7 @@
         <v>44930</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1520,7 +1537,7 @@
         <v>30920</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1549,7 +1566,7 @@
         <v>9891</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1578,7 +1595,7 @@
         <v>7826</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1607,7 +1624,7 @@
         <v>56817</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1653,7 @@
         <v>79289</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1665,7 +1682,7 @@
         <v>47296</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1711,7 @@
         <v>68995</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1723,7 +1740,7 @@
         <v>145587</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1752,7 +1769,7 @@
         <v>76483</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1781,7 +1798,7 @@
         <v>109889</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1810,7 +1827,7 @@
         <v>9027</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1839,7 +1856,7 @@
         <v>7521</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1868,7 +1885,7 @@
         <v>121412</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1897,7 +1914,7 @@
         <v>47831</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1926,7 +1943,7 @@
         <v>48798</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1955,7 +1972,7 @@
         <v>69273</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1984,7 +2001,7 @@
         <v>40975</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -2013,7 +2030,7 @@
         <v>68782</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2042,7 +2059,7 @@
         <v>96184</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2071,7 +2088,7 @@
         <v>44966</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2100,7 +2117,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2129,7 +2146,7 @@
         <v>30225</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2158,7 +2175,7 @@
         <v>75955</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2187,7 +2204,7 @@
         <v>41328</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2216,7 +2233,7 @@
         <v>262134</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2245,7 +2262,7 @@
         <v>82096</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2274,7 +2291,7 @@
         <v>9267</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2303,7 +2320,7 @@
         <v>39780</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2332,7 +2349,7 @@
         <v>66570</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2361,7 +2378,7 @@
         <v>24070</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2390,7 +2407,7 @@
         <v>54464</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2417,6 +2434,332 @@
       </c>
       <c r="I51">
         <v>97203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="29">
+        <v>1</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="26">
+        <v>36161</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25">
+        <v>0</v>
+      </c>
+      <c r="I4" s="25">
+        <v>3121.5468319920351</v>
+      </c>
+      <c r="J4" s="30">
+        <v>40853</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="29">
+        <v>2</v>
+      </c>
+      <c r="E5" s="29">
+        <v>2001</v>
+      </c>
+      <c r="F5" s="26">
+        <v>36526</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25">
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="I5" s="25">
+        <v>-1624.4125246305759</v>
+      </c>
+      <c r="J5" s="30">
+        <v>40853.041666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="29">
+        <v>3</v>
+      </c>
+      <c r="E6" s="29">
+        <v>2002</v>
+      </c>
+      <c r="F6" s="26">
+        <v>36892</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="25">
+        <v>1.0986122886681098</v>
+      </c>
+      <c r="I6" s="25">
+        <v>-3037.6986982328153</v>
+      </c>
+      <c r="J6" s="30">
+        <v>40853.083333333336</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="29">
+        <v>4</v>
+      </c>
+      <c r="E7" s="29">
+        <v>2003</v>
+      </c>
+      <c r="F7" s="26">
+        <v>37257</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="25">
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="I7" s="25">
+        <v>4421.4613537295108</v>
+      </c>
+      <c r="J7" s="30">
+        <v>40853.125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="29">
+        <v>5</v>
+      </c>
+      <c r="E8" s="29">
+        <v>2004</v>
+      </c>
+      <c r="F8" s="26">
+        <v>37622</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="25">
+        <v>1.6094379124341003</v>
+      </c>
+      <c r="I8" s="25">
+        <v>5907.2342279766544</v>
+      </c>
+      <c r="J8" s="30">
+        <v>40853.166666666664</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="29">
+        <v>6</v>
+      </c>
+      <c r="E9" s="29">
+        <v>2005</v>
+      </c>
+      <c r="F9" s="26">
+        <v>37987</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="25">
+        <v>1.791759469228055</v>
+      </c>
+      <c r="I9" s="25">
+        <v>14338.644991521463</v>
+      </c>
+      <c r="J9" s="30">
+        <v>40853.208333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="29">
+        <v>7</v>
+      </c>
+      <c r="E10" s="29">
+        <v>2006</v>
+      </c>
+      <c r="F10" s="26">
+        <v>38353</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="25">
+        <v>1.9459101490553132</v>
+      </c>
+      <c r="I10" s="25">
+        <v>12782.030353787637</v>
+      </c>
+      <c r="J10" s="30">
+        <v>40853.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="29">
+        <v>8</v>
+      </c>
+      <c r="E11" s="29">
+        <v>2007</v>
+      </c>
+      <c r="F11" s="26">
+        <v>38718</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="25">
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="I11" s="25">
+        <v>-11000.620182831051</v>
+      </c>
+      <c r="J11" s="30">
+        <v>40853.291666666664</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="29">
+        <v>9</v>
+      </c>
+      <c r="E12" s="29">
+        <v>2008</v>
+      </c>
+      <c r="F12" s="26">
+        <v>39083</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="25">
+        <v>2.1972245773362196</v>
+      </c>
+      <c r="I12" s="25">
+        <v>-10842.879724285254</v>
+      </c>
+      <c r="J12" s="30">
+        <v>40853.333333333336</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="29">
+        <v>10</v>
+      </c>
+      <c r="E13" s="29">
+        <v>2009</v>
+      </c>
+      <c r="F13" s="26">
+        <v>39448</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" s="25">
+        <v>2.3025850929940459</v>
+      </c>
+      <c r="I13" s="25">
+        <v>16340.029557637967</v>
+      </c>
+      <c r="J13" s="30">
+        <v>40853.375</v>
       </c>
     </row>
   </sheetData>
@@ -2425,21 +2768,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -2459,7 +2802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>39814</v>
       </c>
@@ -2479,7 +2822,7 @@
         <v>39814.042372685188</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>39845</v>
       </c>
@@ -2499,7 +2842,7 @@
         <v>39845.084745370368</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>39873</v>
       </c>
@@ -2520,7 +2863,7 @@
         <v>39873.127117939817</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>39904</v>
       </c>
@@ -2541,7 +2884,7 @@
         <v>39904.169490567132</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>39934</v>
       </c>
@@ -2562,7 +2905,7 @@
         <v>39934.211863194447</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>39965</v>
       </c>
@@ -2583,7 +2926,7 @@
         <v>39965.254235821762</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>39995</v>
       </c>
@@ -2604,7 +2947,7 @@
         <v>39995.296608449076</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>40026</v>
       </c>
@@ -2625,7 +2968,7 @@
         <v>40026.338981076391</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>40057</v>
       </c>
@@ -2646,7 +2989,7 @@
         <v>40057.381353703706</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>40087</v>
       </c>
@@ -2667,7 +3010,7 @@
         <v>40087.423726331021</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>40118</v>
       </c>
@@ -2688,7 +3031,7 @@
         <v>40118.466098958335</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>40148</v>
       </c>
@@ -2716,16 +3059,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -2739,12 +3082,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -2752,7 +3095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>82</v>
       </c>
@@ -2760,7 +3103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>83</v>
       </c>
@@ -2768,7 +3111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>11</v>
       </c>
@@ -2779,35 +3122,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="6" customWidth="1"/>
     <col min="2" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="7" customFormat="1">
+    <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>87</v>
       </c>
@@ -2821,7 +3164,7 @@
       <c r="I4"/>
       <c r="J4"/>
     </row>
-    <row r="5" spans="1:15" s="7" customFormat="1">
+    <row r="5" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -2837,7 +3180,7 @@
         <v>484152</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="7" customFormat="1">
+    <row r="6" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6"/>
       <c r="E6"/>
@@ -2847,29 +3190,29 @@
       <c r="I6"/>
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
     </row>
-    <row r="8" spans="1:15" s="7" customFormat="1" ht="12" customHeight="1">
+    <row r="8" spans="1:15" s="7" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
     </row>
-    <row r="9" spans="1:15" s="7" customFormat="1">
+    <row r="9" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="10" t="s">
         <v>89</v>
@@ -2904,7 +3247,7 @@
       <c r="N9"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>98</v>
       </c>
@@ -2936,7 +3279,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -2948,7 +3291,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="6" t="s">
         <v>100</v>
@@ -2978,7 +3321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>40179</v>
       </c>
@@ -3018,7 +3361,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>40210</v>
       </c>
@@ -3058,7 +3401,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>40238</v>
       </c>
@@ -3098,7 +3441,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>40269</v>
       </c>
@@ -3138,7 +3481,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>40299</v>
       </c>
@@ -3178,7 +3521,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>40330</v>
       </c>
@@ -3218,7 +3561,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>40360</v>
       </c>
@@ -3258,7 +3601,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>40391</v>
       </c>
@@ -3298,7 +3641,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>40422</v>
       </c>
@@ -3338,7 +3681,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>40452</v>
       </c>
@@ -3378,7 +3721,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>40483</v>
       </c>
@@ -3418,7 +3761,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>40513</v>
       </c>
@@ -3458,7 +3801,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>40544</v>
       </c>
@@ -3498,7 +3841,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>40575</v>
       </c>
@@ -3538,7 +3881,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>40603</v>
       </c>
@@ -3578,7 +3921,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>40634</v>
       </c>
@@ -3618,7 +3961,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>40664</v>
       </c>
@@ -3658,7 +4001,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>40695</v>
       </c>
@@ -3698,7 +4041,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>40725</v>
       </c>
@@ -3738,7 +4081,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>40756</v>
       </c>
@@ -3778,7 +4121,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>40787</v>
       </c>
@@ -3818,7 +4161,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>40817</v>
       </c>
@@ -3858,7 +4201,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>40848</v>
       </c>
@@ -3898,7 +4241,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>40878</v>
       </c>
@@ -3948,46 +4291,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3998,26 +4341,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>3</v>
       </c>
@@ -4025,7 +4368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>5</v>
       </c>
@@ -4037,16 +4380,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -4057,7 +4400,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -4069,7 +4412,7 @@
         <v>2010-1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2010</v>
       </c>
@@ -4081,7 +4424,7 @@
         <v>2010-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -4099,20 +4442,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -4132,7 +4475,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>39814</v>
       </c>
@@ -4152,7 +4495,7 @@
         <v>39814.042372685188</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>39845</v>
       </c>
@@ -4172,7 +4515,7 @@
         <v>39845.084745370368</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>39873</v>
       </c>
@@ -4193,7 +4536,7 @@
         <v>39873.127117939817</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>39904</v>
       </c>
@@ -4214,7 +4557,7 @@
         <v>39904.169490567132</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>39934</v>
       </c>
@@ -4235,7 +4578,7 @@
         <v>39934.211863194447</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="e">
         <v>#N/A</v>
       </c>
@@ -4256,7 +4599,7 @@
         <v>39965.254235821762</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>39995</v>
       </c>
@@ -4277,7 +4620,7 @@
         <v>39995.296608449076</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>40026</v>
       </c>
@@ -4298,7 +4641,7 @@
         <v>40026.338981076391</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>40057</v>
       </c>
@@ -4319,7 +4662,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>40087</v>
       </c>
@@ -4340,7 +4683,7 @@
         <v>40087.423726331021</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>40118</v>
       </c>
@@ -4360,7 +4703,7 @@
         <v>40118.466098958335</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>40148</v>
       </c>
@@ -4387,52 +4730,52 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:10">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="22" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>111</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>1</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>2000</v>
       </c>
       <c r="F4" s="1">
@@ -4447,21 +4790,21 @@
       <c r="I4">
         <v>3121.5468319920351</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="23">
         <v>40853</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="22" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
         <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>2</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>2001</v>
       </c>
       <c r="F5" s="1">
@@ -4476,21 +4819,21 @@
       <c r="I5">
         <v>-1624.4125246305759</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="23">
         <v>40853.041666666664</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>115</v>
       </c>
       <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>3</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>2002</v>
       </c>
       <c r="F6" s="1">
@@ -4505,21 +4848,21 @@
       <c r="I6">
         <v>-3037.6986982328153</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="23">
         <v>40853.083333333336</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>4</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>2003</v>
       </c>
       <c r="F7" s="1">
@@ -4534,21 +4877,21 @@
       <c r="I7">
         <v>4421.4613537295108</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="23">
         <v>40853.125</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="22" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>117</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>5</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>2004</v>
       </c>
       <c r="F8" s="1">
@@ -4563,21 +4906,21 @@
       <c r="I8">
         <v>5907.2342279766544</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="23">
         <v>40853.166666666664</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>118</v>
       </c>
       <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>6</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>2005</v>
       </c>
       <c r="F9" s="1">
@@ -4592,21 +4935,21 @@
       <c r="I9">
         <v>14338.644991521463</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="23">
         <v>40853.208333333336</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="22" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
         <v>119</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>7</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>2006</v>
       </c>
       <c r="F10" s="1">
@@ -4621,21 +4964,21 @@
       <c r="I10">
         <v>12782.030353787637</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="23">
         <v>40853.25</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="22" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>120</v>
       </c>
       <c r="C11" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <v>8</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <v>2007</v>
       </c>
       <c r="F11" s="1">
@@ -4650,21 +4993,21 @@
       <c r="I11">
         <v>-11000.620182831051</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="23">
         <v>40853.291666666664</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="22" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>9</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <v>2008</v>
       </c>
       <c r="F12" s="1">
@@ -4679,21 +5022,21 @@
       <c r="I12">
         <v>-10842.879724285254</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="23">
         <v>40853.333333333336</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="22" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>122</v>
       </c>
       <c r="C13" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>10</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>2009</v>
       </c>
       <c r="F13" s="1">
@@ -4708,7 +5051,7 @@
       <c r="I13">
         <v>16340.029557637967</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="23">
         <v>40853.375</v>
       </c>
     </row>

</xml_diff>